<commit_message>
chore: persist prospect eval results
</commit_message>
<xml_diff>
--- a/src/main/resources/files/prospect-ok.xlsx
+++ b/src/main/resources/files/prospect-ok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afryan/IdeaProjects/bpartners-api/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5660E66B-8C90-2347-87B8-EA415B5EB483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3104C2AF-DCEF-294F-A5AC-7E7EA21D805F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="218">
   <si>
     <t>website</t>
   </si>
@@ -713,6 +713,13 @@
   <si>
     <t>restaurant</t>
   </si>
+  <si>
+    <t>ID du propriétaire du prospect 
+(ID Account Holder)</t>
+  </si>
+  <si>
+    <t>b33e6eb0-e262-4596-a91f-20c6a7bfd343</t>
+  </si>
 </sst>
 </file>
 
@@ -721,7 +728,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,8 +807,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,8 +869,14 @@
         <bgColor rgb="FFF7CAAC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor rgb="FFF7CAAC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1000,12 +1019,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1170,6 +1224,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1399,7 +1465,7 @@
   <dimension ref="A1:AN7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:AD1"/>
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1491,9 @@
     <col min="26" max="26" width="20.5" customWidth="1"/>
     <col min="27" max="27" width="24.1640625" customWidth="1"/>
     <col min="28" max="28" width="11.5" style="31" customWidth="1"/>
-    <col min="29" max="32" width="14.5" style="31"/>
+    <col min="29" max="30" width="14.5" style="31"/>
+    <col min="31" max="31" width="33.83203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5" style="31"/>
     <col min="33" max="33" width="22.33203125" style="31" customWidth="1"/>
     <col min="34" max="34" width="21.5" style="31" customWidth="1"/>
     <col min="35" max="35" width="23.5" style="31" customWidth="1"/>
@@ -1527,6 +1595,9 @@
       <c r="AD1" s="43">
         <v>29</v>
       </c>
+      <c r="AE1" s="43">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:40" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -1619,7 +1690,9 @@
       <c r="AD2" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="AE2" s="32"/>
+      <c r="AE2" s="60" t="s">
+        <v>216</v>
+      </c>
       <c r="AF2" s="32"/>
       <c r="AG2" s="32"/>
       <c r="AH2" s="32"/>
@@ -1704,8 +1777,10 @@
       <c r="AA3" s="27"/>
       <c r="AB3" s="26"/>
       <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="34"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="61" t="s">
+        <v>217</v>
+      </c>
       <c r="AF3" s="34"/>
       <c r="AG3" s="33"/>
       <c r="AH3" s="34"/>
@@ -1784,8 +1859,10 @@
       <c r="AA4" s="27"/>
       <c r="AB4" s="26"/>
       <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="34"/>
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="61" t="s">
+        <v>217</v>
+      </c>
       <c r="AF4" s="34"/>
       <c r="AG4" s="33"/>
       <c r="AH4" s="34"/>
@@ -1862,8 +1939,10 @@
       <c r="AC5" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="33"/>
+      <c r="AD5" s="59"/>
+      <c r="AE5" s="61" t="s">
+        <v>217</v>
+      </c>
       <c r="AF5" s="33"/>
       <c r="AG5" s="33"/>
       <c r="AH5" s="33"/>
@@ -1954,8 +2033,10 @@
       </c>
       <c r="AB6" s="26"/>
       <c r="AC6" s="27"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="33"/>
+      <c r="AD6" s="58"/>
+      <c r="AE6" s="61" t="s">
+        <v>217</v>
+      </c>
       <c r="AF6" s="33"/>
       <c r="AG6" s="33"/>
       <c r="AH6" s="33"/>
@@ -2042,8 +2123,10 @@
       <c r="AA7" s="26"/>
       <c r="AB7" s="26"/>
       <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="34"/>
+      <c r="AD7" s="59"/>
+      <c r="AE7" s="61" t="s">
+        <v>217</v>
+      </c>
       <c r="AF7" s="34"/>
       <c r="AG7" s="33"/>
       <c r="AH7" s="34"/>
@@ -2055,6 +2138,7 @@
       <c r="AN7" s="33"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U6:U7 U3 I3:I7 P3:T7 AB3:AB7" xr:uid="{5927C8BD-C5E0-BD4C-9A04-5AA2141EF2DB}">
       <formula1>"Yes,No"</formula1>

</xml_diff>